<commit_message>
Vectorized Integral for mW Transform
</commit_message>
<xml_diff>
--- a/src/ifrost/models/2layerver.xlsx
+++ b/src/ifrost/models/2layerver.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="15" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="3">
   <si>
     <t>Frequency</t>
   </si>
@@ -67,7 +67,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -91,936 +91,1090 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>472331.61071791139</v>
+        <v>309216.72195662616</v>
       </c>
       <c r="B2" s="0">
-        <v>0.00014375062042537722</v>
+        <v>6.432740354873052e-05</v>
       </c>
       <c r="C2" s="0">
-        <v>0.0031577844756663382</v>
+        <v>0.0020755061388499827</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>486842.77447561914</v>
+        <v>318716.60379200469</v>
       </c>
       <c r="B3" s="0">
-        <v>0.0001521828017836304</v>
+        <v>6.8152880961863484e-05</v>
       </c>
       <c r="C3" s="0">
-        <v>0.0032535507148257104</v>
+        <v>0.0021388168144818006</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>501799.75610539969</v>
+        <v>328508.34485904151</v>
       </c>
       <c r="B4" s="0">
-        <v>0.00016109761627566697</v>
+        <v>7.220254442769597e-05</v>
       </c>
       <c r="C4" s="0">
-        <v>0.0033521639346038678</v>
+        <v>0.0022040379556319332</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>517216.25220515375</v>
+        <v>338600.91177569894</v>
       </c>
       <c r="B5" s="0">
-        <v>0.00017052460677231793</v>
+        <v>7.6489237177265558e-05</v>
       </c>
       <c r="C5" s="0">
-        <v>0.0034537104279688761</v>
+        <v>0.0022712260248251241</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>533106.38016523072</v>
+        <v>349003.54663602181</v>
       </c>
       <c r="B6" s="0">
-        <v>0.00018049075475730855</v>
+        <v>8.1026512618931942e-05</v>
       </c>
       <c r="C6" s="0">
-        <v>0.0035582697254512383</v>
+        <v>0.0023404387556790296</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>549484.69109618501</v>
+        <v>359725.77547342377</v>
       </c>
       <c r="B7" s="0">
-        <v>0.00019102582624647943</v>
+        <v>8.582906552427731e-05</v>
       </c>
       <c r="C7" s="0">
-        <v>0.0036659268008959133</v>
+        <v>0.0024117356960728785</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>566366.18315370637</v>
+        <v>370777.41698399116</v>
       </c>
       <c r="B8" s="0">
-        <v>0.00020216114098781188</v>
+        <v>9.0911233286514805e-05</v>
       </c>
       <c r="C8" s="0">
-        <v>0.0037767686063475098</v>
+        <v>0.0024851771570681531</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>583766.31527291727</v>
+        <v>382168.59151778265</v>
       </c>
       <c r="B9" s="0">
-        <v>0.00021392964621430873</v>
+        <v>9.628929535888172e-05</v>
       </c>
       <c r="C9" s="0">
-        <v>0.003890884161417888</v>
+        <v>0.0025608259558559379</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>601701.02132463246</v>
+        <v>393909.73034636519</v>
       </c>
       <c r="B10" s="0">
-        <v>0.00022636599330404152</v>
+        <v>0.00010198003934313179</v>
       </c>
       <c r="C10" s="0">
-        <v>0.0040083645955917785</v>
+        <v>0.0026387462810003441</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>620186.72470652265</v>
+        <v>406011.58521507186</v>
       </c>
       <c r="B11" s="0">
-        <v>0.0002395066174141696</v>
+        <v>0.00010800116988670507</v>
       </c>
       <c r="C11" s="0">
-        <v>0.0041293031787005769</v>
+        <v>0.002719004031060047</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>639240.35338255786</v>
+        <v>418485.23818872619</v>
       </c>
       <c r="B12" s="0">
-        <v>0.00025338982015380595</v>
+        <v>0.0001143713584827451</v>
       </c>
       <c r="C12" s="0">
-        <v>0.004253795346553165</v>
+        <v>0.0028016668489241076</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>658879.3553844993</v>
+        <v>431342.11179985252</v>
       </c>
       <c r="B13" s="0">
-        <v>0.00026805585535690673</v>
+        <v>0.00012111030052864789</v>
       </c>
       <c r="C13" s="0">
-        <v>0.0043819387235547918</v>
+        <v>0.0028868041560145405</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>679121.71478963224</v>
+        <v>444593.97950866388</v>
       </c>
       <c r="B14" s="0">
-        <v>0.00028354701801391451</v>
+        <v>0.00012823879332262182</v>
       </c>
       <c r="C14" s="0">
-        <v>0.0045138331428216496</v>
+        <v>0.0029744871862813866</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>699985.96818937606</v>
+        <v>458252.97648440139</v>
       </c>
       <c r="B15" s="0">
-        <v>0.00029990773641766494</v>
+        <v>0.00013577891945109117</v>
       </c>
       <c r="C15" s="0">
-        <v>0.0046495806638743213</v>
+        <v>0.0030647890199106335</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>721491.22166384792</v>
+        <v>472331.61071791139</v>
       </c>
       <c r="B16" s="0">
-        <v>0.00031718466757519399</v>
+        <v>0.00014375062042537722</v>
       </c>
       <c r="C16" s="0">
-        <v>0.0047892855878309435</v>
+        <v>0.0031577844756663382</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>743657.16827792197</v>
+        <v>486842.77447561914</v>
       </c>
       <c r="B17" s="0">
-        <v>0.00033542679593511268</v>
+        <v>0.0001521828017836304</v>
       </c>
       <c r="C17" s="0">
-        <v>0.0049330544699482792</v>
+        <v>0.0032535507148257104</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>766504.10611482</v>
+        <v>501799.75610539969</v>
       </c>
       <c r="B18" s="0">
-        <v>0.00035468553547680237</v>
+        <v>0.00016109761627566697</v>
       </c>
       <c r="C18" s="0">
-        <v>0.0050809961293207043</v>
+        <v>0.0033521639346038678</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>790052.95686372812</v>
+        <v>517216.25220515375</v>
       </c>
       <c r="B19" s="0">
-        <v>0.00037501483520848485</v>
+        <v>0.00017052460677231793</v>
       </c>
       <c r="C19" s="0">
-        <v>0.0052332216555228336</v>
+        <v>0.0034537104279688761</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>814325.28497847228</v>
+        <v>533106.38016523072</v>
       </c>
       <c r="B20" s="0">
-        <v>0.00039647128812335495</v>
+        <v>0.00018049075475730855</v>
       </c>
       <c r="C20" s="0">
-        <v>0.0053898444119644742</v>
+        <v>0.0035582697254512383</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>839343.31742479513</v>
+        <v>549484.69109618501</v>
       </c>
       <c r="B21" s="0">
-        <v>0.00041911424367302279</v>
+        <v>0.00019102582624647943</v>
       </c>
       <c r="C21" s="0">
-        <v>0.0055509800357121742</v>
+        <v>0.0036659268008959133</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>865129.9640343166</v>
+        <v>566366.18315370637</v>
       </c>
       <c r="B22" s="0">
-        <v>0.0004430059238395113</v>
+        <v>0.00020216114098781188</v>
       </c>
       <c r="C22" s="0">
-        <v>0.0057167464335190696</v>
+        <v>0.0037767686063475098</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>891708.83848381718</v>
+        <v>583766.31527291727</v>
       </c>
       <c r="B23" s="0">
-        <v>0.00046821154293434273</v>
+        <v>0.00021392964621430873</v>
       </c>
       <c r="C23" s="0">
-        <v>0.0058872637737930073</v>
+        <v>0.003890884161417888</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>919104.27991905471</v>
+        <v>601701.02132463246</v>
       </c>
       <c r="B24" s="0">
-        <v>0.0004947994313501189</v>
+        <v>0.00022636599330404152</v>
       </c>
       <c r="C24" s="0">
-        <v>0.0060626544742218126</v>
+        <v>0.0040083645955917785</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>947341.37524291955</v>
+        <v>620186.72470652265</v>
       </c>
       <c r="B25" s="0">
-        <v>0.00052284116369434553</v>
+        <v>0.0002395066174141696</v>
       </c>
       <c r="C25" s="0">
-        <v>0.0062430431847638546</v>
+        <v>0.0041293031787005769</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>976445.98208832543</v>
+        <v>639240.35338255786</v>
       </c>
       <c r="B26" s="0">
-        <v>0.00055241169218206334</v>
+        <v>0.00025338982015380595</v>
       </c>
       <c r="C26" s="0">
-        <v>0.0064285567657015458</v>
+        <v>0.004253795346553165</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>1006444.7524969012</v>
+        <v>658879.3553844993</v>
       </c>
       <c r="B27" s="0">
-        <v>0.00058358948720476354</v>
+        <v>0.00026805585535690673</v>
       </c>
       <c r="C27" s="0">
-        <v>0.0066193242604458014</v>
+        <v>0.0043819387235547918</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>1037365.1573251319</v>
+        <v>679121.71478963224</v>
       </c>
       <c r="B28" s="0">
-        <v>0.00061645260130544681</v>
+        <v>0.00028354701801391451</v>
       </c>
       <c r="C28" s="0">
-        <v>0.0068154744452149354</v>
+        <v>0.0045138331428216496</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>1069235.5114003231</v>
+        <v>699985.96818937606</v>
       </c>
       <c r="B29" s="0">
-        <v>0.00065109525787955308</v>
+        <v>0.00029990773641766494</v>
       </c>
       <c r="C29" s="0">
-        <v>0.0070171456822511876</v>
+        <v>0.0046495806638743213</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>1102084.9994494151</v>
+        <v>721491.22166384792</v>
       </c>
       <c r="B30" s="0">
-        <v>0.00068759937123928313</v>
+        <v>0.00031718466757519399</v>
       </c>
       <c r="C30" s="0">
-        <v>0.007224469090518602</v>
+        <v>0.0047892855878309435</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>1135943.702824394</v>
+        <v>743657.16827792197</v>
       </c>
       <c r="B31" s="0">
-        <v>0.00072606483077610048</v>
+        <v>0.00033542679593511268</v>
       </c>
       <c r="C31" s="0">
-        <v>0.0074375840194043069</v>
+        <v>0.0049330544699482792</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>1170842.6270487718</v>
+        <v>766504.10611482</v>
       </c>
       <c r="B32" s="0">
-        <v>0.00076657884627426916</v>
+        <v>0.00035468553547680237</v>
       </c>
       <c r="C32" s="0">
-        <v>0.0076566262357920115</v>
+        <v>0.0050809961293207043</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>1206813.7302103522</v>
+        <v>790052.95686372812</v>
       </c>
       <c r="B33" s="0">
-        <v>0.00080925863193886049</v>
+        <v>0.00037501483520848485</v>
       </c>
       <c r="C33" s="0">
-        <v>0.0078817463081357411</v>
+        <v>0.0052332216555228336</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>1243889.9522263105</v>
+        <v>814325.28497847228</v>
       </c>
       <c r="B34" s="0">
-        <v>0.00085420436910654503</v>
+        <v>0.00039647128812335495</v>
       </c>
       <c r="C34" s="0">
-        <v>0.0081130803746709973</v>
+        <v>0.0053898444119644742</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>1282105.2450073464</v>
+        <v>839343.31742479513</v>
       </c>
       <c r="B35" s="0">
-        <v>0.00090152803123512762</v>
+        <v>0.00041911424367302279</v>
       </c>
       <c r="C35" s="0">
-        <v>0.0083507737040542825</v>
+        <v>0.0055509800357121742</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>1321494.6035485617</v>
+        <v>865129.9640343166</v>
       </c>
       <c r="B36" s="0">
-        <v>0.00095133788532609923</v>
+        <v>0.0004430059238395113</v>
       </c>
       <c r="C36" s="0">
-        <v>0.0085949652175620235</v>
+        <v>0.0057167464335190696</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>1362094.0979755244</v>
+        <v>891708.83848381718</v>
       </c>
       <c r="B37" s="0">
-        <v>0.0010037691082924517</v>
+        <v>0.00046821154293434273</v>
       </c>
       <c r="C37" s="0">
-        <v>0.0088458210535663669</v>
+        <v>0.0058872637737930073</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>1403940.9065748637</v>
+        <v>919104.27991905471</v>
       </c>
       <c r="B38" s="0">
-        <v>0.0010589354145216481</v>
+        <v>0.0004947994313501189</v>
       </c>
       <c r="C38" s="0">
-        <v>0.0091034723031923545</v>
+        <v>0.0060626544742218126</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>1447073.3498396436</v>
+        <v>947341.37524291955</v>
       </c>
       <c r="B39" s="0">
-        <v>0.0011169800073005257</v>
+        <v>0.00052284116369434553</v>
       </c>
       <c r="C39" s="0">
-        <v>0.0093680855115546458</v>
+        <v>0.0062430431847638546</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>1491530.9255606951</v>
+        <v>976445.98208832543</v>
       </c>
       <c r="B40" s="0">
-        <v>0.0011780359883842013</v>
+        <v>0.00055241169218206334</v>
       </c>
       <c r="C40" s="0">
-        <v>0.0096398035135114978</v>
+        <v>0.0064285567657015458</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>1537354.3449960351</v>
+        <v>1006444.7524969012</v>
       </c>
       <c r="B41" s="0">
-        <v>0.0012422349878499217</v>
+        <v>0.00058358948720476354</v>
       </c>
       <c r="C41" s="0">
-        <v>0.0099187678051892939</v>
+        <v>0.0066193242604458014</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>1584585.570151503</v>
+        <v>1037365.1573251319</v>
       </c>
       <c r="B42" s="0">
-        <v>0.0013097391659458557</v>
+        <v>0.00061645260130544681</v>
       </c>
       <c r="C42" s="0">
-        <v>0.010205156752153324</v>
+        <v>0.0068154744452149354</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>1633267.8522067301</v>
+        <v>1069235.5114003231</v>
       </c>
       <c r="B43" s="0">
-        <v>0.001380701959479704</v>
+        <v>0.00065109525787955308</v>
       </c>
       <c r="C43" s="0">
-        <v>0.010499117368543472</v>
+        <v>0.0070171456822511876</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>1683445.771121681</v>
+        <v>1102084.9994494151</v>
       </c>
       <c r="B44" s="0">
-        <v>0.0014552748817301064</v>
+        <v>0.00068759937123928313</v>
       </c>
       <c r="C44" s="0">
-        <v>0.010800788712367296</v>
+        <v>0.007224469090518602</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>1735165.2764599686</v>
+        <v>1135943.702824394</v>
       </c>
       <c r="B45" s="0">
-        <v>0.0015336346145457566</v>
+        <v>0.00072606483077610048</v>
       </c>
       <c r="C45" s="0">
-        <v>0.011110348427900534</v>
+        <v>0.0074375840194043069</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>1788473.729466381</v>
+        <v>1170842.6270487718</v>
       </c>
       <c r="B46" s="0">
-        <v>0.0016159547097790584</v>
+        <v>0.00076657884627426916</v>
       </c>
       <c r="C46" s="0">
-        <v>0.011427939341074372</v>
+        <v>0.0076566262357920115</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>1843419.9464371197</v>
+        <v>1206813.7302103522</v>
       </c>
       <c r="B47" s="0">
-        <v>0.0017023918934662638</v>
+        <v>0.00080925863193886049</v>
       </c>
       <c r="C47" s="0">
-        <v>0.011753714913661747</v>
+        <v>0.0078817463081357411</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>1900054.2434224843</v>
+        <v>1243889.9522263105</v>
       </c>
       <c r="B48" s="0">
-        <v>0.0017931664427524787</v>
+        <v>0.00085420436910654503</v>
       </c>
       <c r="C48" s="0">
-        <v>0.012087845073539258</v>
+        <v>0.0081130803746709973</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>1958428.4823029297</v>
+        <v>1282105.2450073464</v>
       </c>
       <c r="B49" s="0">
-        <v>0.0018884440015224072</v>
+        <v>0.00090152803123512762</v>
       </c>
       <c r="C49" s="0">
-        <v>0.012430472457349302</v>
+        <v>0.0083507737040542825</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>2018596.1182806739</v>
+        <v>1321494.6035485617</v>
       </c>
       <c r="B50" s="0">
-        <v>0.0019884421387292291</v>
+        <v>0.00095133788532609923</v>
       </c>
       <c r="C50" s="0">
-        <v>0.012781754259314809</v>
+        <v>0.0085949652175620235</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>2080612.2488303988</v>
+        <v>1362094.0979755244</v>
       </c>
       <c r="B51" s="0">
-        <v>0.0020933568425876474</v>
+        <v>0.0010037691082924517</v>
       </c>
       <c r="C51" s="0">
-        <v>0.013141840261078105</v>
+        <v>0.0088458210535663669</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>2144533.6641537999</v>
+        <v>1403940.9065748637</v>
       </c>
       <c r="B52" s="0">
-        <v>0.0022034129277448771</v>
+        <v>0.0010589354145216481</v>
       </c>
       <c r="C52" s="0">
-        <v>0.013510891862414035</v>
+        <v>0.0091034723031923545</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>2210418.899184233</v>
+        <v>1447073.3498396436</v>
       </c>
       <c r="B53" s="0">
-        <v>0.0023188240598180513</v>
+        <v>0.0011169800073005257</v>
       </c>
       <c r="C53" s="0">
-        <v>0.013889055403717588</v>
+        <v>0.0093680855115546458</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>2278328.2871890743</v>
+        <v>1491530.9255606951</v>
       </c>
       <c r="B54" s="0">
-        <v>0.0024398189565490382</v>
+        <v>0.0011780359883842013</v>
       </c>
       <c r="C54" s="0">
-        <v>0.014276477303922957</v>
+        <v>0.0096398035135114978</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>2348324.0150188669</v>
+        <v>1537354.3449960351</v>
       </c>
       <c r="B55" s="0">
-        <v>0.0025666364781297092</v>
+        <v>0.0012422349878499217</v>
       </c>
       <c r="C55" s="0">
-        <v>0.014673305131220046</v>
+        <v>0.0099187678051892939</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>2420470.1800538553</v>
+        <v>1584585.570151503</v>
       </c>
       <c r="B56" s="0">
-        <v>0.0026995077038295245</v>
+        <v>0.0013097391659458557</v>
       </c>
       <c r="C56" s="0">
-        <v>0.015079683531840936</v>
+        <v>0.010205156752153324</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>2494832.8489000583</v>
+        <v>1633267.8522067301</v>
       </c>
       <c r="B57" s="0">
-        <v>0.0028387145020227615</v>
+        <v>0.001380701959479704</v>
       </c>
       <c r="C57" s="0">
-        <v>0.015495756366620185</v>
+        <v>0.010499117368543472</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>2571480.1178886271</v>
+        <v>1683445.771121681</v>
       </c>
       <c r="B58" s="0">
-        <v>0.0029844911984264989</v>
+        <v>0.0014552748817301064</v>
       </c>
       <c r="C58" s="0">
-        <v>0.015921661906115551</v>
+        <v>0.010800788712367296</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>2650482.1754338653</v>
+        <v>1735165.2764599686</v>
       </c>
       <c r="B59" s="0">
-        <v>0.0031371134545994514</v>
+        <v>0.0015336346145457566</v>
       </c>
       <c r="C59" s="0">
-        <v>0.016357531170786661</v>
+        <v>0.011110348427900534</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>2731911.3663070891</v>
+        <v>1788473.729466381</v>
       </c>
       <c r="B60" s="0">
-        <v>0.0032968628765485558</v>
+        <v>0.0016159547097790584</v>
       </c>
       <c r="C60" s="0">
-        <v>0.016803502681549985</v>
+        <v>0.011427939341074372</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>2815842.2578850854</v>
+        <v>1843419.9464371197</v>
       </c>
       <c r="B61" s="0">
-        <v>0.0034640227709706656</v>
+        <v>0.0017023918934662638</v>
       </c>
       <c r="C61" s="0">
-        <v>0.017259696478195859</v>
+        <v>0.011753714913661747</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>2902351.7084339014</v>
+        <v>1900054.2434224843</v>
       </c>
       <c r="B62" s="0">
-        <v>0.0036388524283729098</v>
+        <v>0.0017931664427524787</v>
       </c>
       <c r="C62" s="0">
-        <v>0.017726231039284595</v>
+        <v>0.012087845073539258</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>2991518.937490481</v>
+        <v>1958428.4823029297</v>
       </c>
       <c r="B63" s="0">
-        <v>0.0038216939060491169</v>
+        <v>0.0018884440015224072</v>
       </c>
       <c r="C63" s="0">
-        <v>0.018203232637930791</v>
+        <v>0.012430472457349302</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>3083425.598406584</v>
+        <v>2018596.1182806739</v>
       </c>
       <c r="B64" s="0">
-        <v>0.0040128265866630625</v>
+        <v>0.0019884421387292291</v>
       </c>
       <c r="C64" s="0">
-        <v>0.018690795573471659</v>
+        <v>0.012781754259314809</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>3178155.8531214464</v>
+        <v>2080612.2488303988</v>
       </c>
       <c r="B65" s="0">
-        <v>0.0042125816886336136</v>
+        <v>0.0020933568425876474</v>
       </c>
       <c r="C65" s="0">
-        <v>0.019189040381150543</v>
+        <v>0.013141840261078105</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>3275796.4492315929</v>
+        <v>2144533.6641537999</v>
       </c>
       <c r="B66" s="0">
-        <v>0.0044212709254043857</v>
+        <v>0.0022034129277448771</v>
       </c>
       <c r="C66" s="0">
-        <v>0.019698080259523201</v>
+        <v>0.013510891862414035</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>3376436.7994284947</v>
+        <v>2210418.899184233</v>
       </c>
       <c r="B67" s="0">
-        <v>0.0046392245438947608</v>
+        <v>0.0023188240598180513</v>
       </c>
       <c r="C67" s="0">
-        <v>0.020217969981141112</v>
+        <v>0.013889055403717588</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>3480169.0633766702</v>
+        <v>2278328.2871890743</v>
       </c>
       <c r="B68" s="0">
-        <v>0.004866792199969789</v>
+        <v>0.0024398189565490382</v>
       </c>
       <c r="C68" s="0">
-        <v>0.020748823804174234</v>
+        <v>0.014276477303922957</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>3587088.232107318</v>
+        <v>2348324.0150188669</v>
       </c>
       <c r="B69" s="0">
-        <v>0.005104299294626944</v>
+        <v>0.0025666364781297092</v>
       </c>
       <c r="C69" s="0">
-        <v>0.021290704022524119</v>
+        <v>0.014673305131220046</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>3697292.2150047128</v>
+        <v>2420470.1800538553</v>
       </c>
       <c r="B70" s="0">
-        <v>0.0053521080759151235</v>
+        <v>0.0026995077038295245</v>
       </c>
       <c r="C70" s="0">
-        <v>0.021843691005800102</v>
+        <v>0.015079683531840936</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>3810881.9294650336</v>
+        <v>2494832.8489000583</v>
       </c>
       <c r="B71" s="0">
-        <v>0.0056105806609877407</v>
+        <v>0.0028387145020227615</v>
       </c>
       <c r="C71" s="0">
-        <v>0.022407827390162827</v>
+        <v>0.015495756366620185</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>3927961.3933097324</v>
+        <v>2571480.1178886271</v>
       </c>
       <c r="B72" s="0">
-        <v>0.0058800803794695697</v>
+        <v>0.0029844911984264989</v>
       </c>
       <c r="C72" s="0">
-        <v>0.022983168126622114</v>
+        <v>0.015921661906115551</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>4048637.8200380574</v>
+        <v>2650482.1754338653</v>
       </c>
       <c r="B73" s="0">
-        <v>0.0061609629830356371</v>
+        <v>0.0031371134545994514</v>
       </c>
       <c r="C73" s="0">
-        <v>0.023569767066138735</v>
+        <v>0.016357531170786661</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>4173021.7170059611</v>
+        <v>2731911.3663070891</v>
       </c>
       <c r="B74" s="0">
-        <v>0.0064536412206358078</v>
+        <v>0.0032968628765485558</v>
       </c>
       <c r="C74" s="0">
-        <v>0.024167643463930358</v>
+        <v>0.016803502681549985</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>4301226.986621324</v>
+        <v>2815842.2578850854</v>
       </c>
       <c r="B75" s="0">
-        <v>0.0067584740060114739</v>
+        <v>0.0034640227709706656</v>
       </c>
       <c r="C75" s="0">
-        <v>0.024776818763393455</v>
+        <v>0.017259696478195859</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>4433371.0306480741</v>
+        <v>2902351.7084339014</v>
       </c>
       <c r="B76" s="0">
-        <v>0.007075844094947957</v>
+        <v>0.0036388524283729098</v>
       </c>
       <c r="C76" s="0">
-        <v>0.025397292712000766</v>
+        <v>0.017726231039284595</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>4569574.8577148868</v>
+        <v>2991518.937490481</v>
       </c>
       <c r="B77" s="0">
-        <v>0.0074061797389542387</v>
+        <v>0.0038216939060491169</v>
       </c>
       <c r="C77" s="0">
-        <v>0.026029071162606308</v>
+        <v>0.018203232637930791</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>4709963.1941267103</v>
+        <v>3083425.598406584</v>
       </c>
       <c r="B78" s="0">
-        <v>0.0077498569819000069</v>
+        <v>0.0040128265866630625</v>
       </c>
       <c r="C78" s="0">
-        <v>0.026672154502528262</v>
+        <v>0.018690795573471659</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>4854664.5980807375</v>
+        <v>3178155.8531214464</v>
       </c>
       <c r="B79" s="0">
-        <v>0.0081072843316619871</v>
+        <v>0.0042125816886336136</v>
       </c>
       <c r="C79" s="0">
-        <v>0.027326482979874965</v>
+        <v>0.019189040381150543</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>5003811.5773913572</v>
+        <v>3275796.4492315929</v>
       </c>
       <c r="B80" s="0">
-        <v>0.0084788780358815551</v>
+        <v>0.0044212709254043857</v>
       </c>
       <c r="C80" s="0">
-        <v>0.02799201931382888</v>
+        <v>0.019698080259523201</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>5157540.7108319095</v>
+        <v>3376436.7994284947</v>
       </c>
       <c r="B81" s="0">
-        <v>0.0088650411417777551</v>
+        <v>0.0046392245438947608</v>
       </c>
       <c r="C81" s="0">
-        <v>0.028668743890503966</v>
+        <v>0.020217969981141112</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>5315992.7732042987</v>
+        <v>3480169.0633766702</v>
       </c>
       <c r="B82" s="0">
-        <v>0.0092661982534570659</v>
+        <v>0.004866792199969789</v>
       </c>
       <c r="C82" s="0">
-        <v>0.029356550874016035</v>
+        <v>0.020748823804174234</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>5479312.8642511582</v>
+        <v>3587088.232107318</v>
       </c>
       <c r="B83" s="0">
-        <v>0.0096827639522085521</v>
+        <v>0.005104299294626944</v>
       </c>
       <c r="C83" s="0">
-        <v>0.030055368488626184</v>
+        <v>0.021290704022524119</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>5647650.5415283814</v>
+        <v>3697292.2150047128</v>
       </c>
       <c r="B84" s="0">
-        <v>0.010115136504452395</v>
+        <v>0.0053521080759151235</v>
       </c>
       <c r="C84" s="0">
-        <v>0.03076508911814587</v>
+        <v>0.021843691005800102</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>5821159.9573598988</v>
+        <v>3810881.9294650336</v>
       </c>
       <c r="B85" s="0">
-        <v>0.010563780454183986</v>
+        <v>0.0056105806609877407</v>
       </c>
       <c r="C85" s="0">
-        <v>0.031485637843218971</v>
+        <v>0.022407827390162827</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0">
+        <v>3927961.3933097324</v>
+      </c>
+      <c r="B86" s="0">
+        <v>0.0058800803794695697</v>
+      </c>
+      <c r="C86" s="0">
+        <v>0.022983168126622114</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0">
+        <v>4048637.8200380574</v>
+      </c>
+      <c r="B87" s="0">
+        <v>0.0061609629830356371</v>
+      </c>
+      <c r="C87" s="0">
+        <v>0.023569767066138735</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0">
+        <v>4173021.7170059611</v>
+      </c>
+      <c r="B88" s="0">
+        <v>0.0064536412206358078</v>
+      </c>
+      <c r="C88" s="0">
+        <v>0.024167643463930358</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0">
+        <v>4301226.986621324</v>
+      </c>
+      <c r="B89" s="0">
+        <v>0.0067584740060114739</v>
+      </c>
+      <c r="C89" s="0">
+        <v>0.024776818763393455</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0">
+        <v>4433371.0306480741</v>
+      </c>
+      <c r="B90" s="0">
+        <v>0.007075844094947957</v>
+      </c>
+      <c r="C90" s="0">
+        <v>0.025397292712000766</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="0">
+        <v>4569574.8577148868</v>
+      </c>
+      <c r="B91" s="0">
+        <v>0.0074061797389542387</v>
+      </c>
+      <c r="C91" s="0">
+        <v>0.026029071162606308</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0">
+        <v>4709963.1941267103</v>
+      </c>
+      <c r="B92" s="0">
+        <v>0.0077498569819000069</v>
+      </c>
+      <c r="C92" s="0">
+        <v>0.026672154502528262</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="0">
+        <v>4854664.5980807375</v>
+      </c>
+      <c r="B93" s="0">
+        <v>0.0081072843316619871</v>
+      </c>
+      <c r="C93" s="0">
+        <v>0.027326482979874965</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0">
+        <v>5003811.5773913572</v>
+      </c>
+      <c r="B94" s="0">
+        <v>0.0084788780358815551</v>
+      </c>
+      <c r="C94" s="0">
+        <v>0.02799201931382888</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="0">
+        <v>5157540.7108319095</v>
+      </c>
+      <c r="B95" s="0">
+        <v>0.0088650411417777551</v>
+      </c>
+      <c r="C95" s="0">
+        <v>0.028668743890503966</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0">
+        <v>5315992.7732042987</v>
+      </c>
+      <c r="B96" s="0">
+        <v>0.0092661982534570659</v>
+      </c>
+      <c r="C96" s="0">
+        <v>0.029356550874016035</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0">
+        <v>5479312.8642511582</v>
+      </c>
+      <c r="B97" s="0">
+        <v>0.0096827639522085521</v>
+      </c>
+      <c r="C97" s="0">
+        <v>0.030055368488626184</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0">
+        <v>5647650.5415283814</v>
+      </c>
+      <c r="B98" s="0">
+        <v>0.010115136504452395</v>
+      </c>
+      <c r="C98" s="0">
+        <v>0.03076508911814587</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0">
+        <v>5821159.9573598988</v>
+      </c>
+      <c r="B99" s="0">
+        <v>0.010563780454183986</v>
+      </c>
+      <c r="C99" s="0">
+        <v>0.031485637843218971</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0">
         <v>6000000.0000000037</v>
       </c>
-      <c r="B86" s="0">
+      <c r="B100" s="0">
         <v>0.011029079046023344</v>
       </c>
-      <c r="C86" s="0">
+      <c r="C100" s="0">
         <v>0.032216832655445567</v>
       </c>
     </row>

</xml_diff>